<commit_message>
separate facies result analysis
</commit_message>
<xml_diff>
--- a/data/exp_raw/johann_batch_preprocessed_part2.xlsx
+++ b/data/exp_raw/johann_batch_preprocessed_part2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/AmmerBatch/data/exp_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcant\Documents\AmmerBatch\data\exp_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9B19F-62EE-6E4E-B33D-595419540CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329EE3A7-BE36-4362-8A0F-B52F4B8148F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="1180" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,11 +179,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -476,8 +478,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,16 +760,16 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -787,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="19" t="s">
         <v>12</v>
       </c>
@@ -798,12 +800,14 @@
       <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>1.2</v>
+      </c>
       <c r="F2" s="18">
         <v>15.339999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
@@ -821,7 +825,7 @@
         <v>17.12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
@@ -839,7 +843,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
@@ -857,7 +861,7 @@
         <v>23.41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="19" t="s">
         <v>16</v>
       </c>
@@ -875,7 +879,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>17</v>
       </c>
@@ -887,13 +891,13 @@
         <v>6</v>
       </c>
       <c r="E7" s="41">
-        <v>15.4</v>
+        <v>7.5</v>
       </c>
       <c r="F7" s="18">
         <v>7.3699999999999992</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="37" t="s">
         <v>18</v>
       </c>
@@ -904,12 +908,14 @@
       <c r="D8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="39">
+        <v>43</v>
+      </c>
       <c r="F8" s="40">
         <v>3.0100000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="37" t="s">
         <v>19</v>
       </c>
@@ -925,7 +931,7 @@
         <v>3.6100000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
@@ -943,7 +949,7 @@
         <v>15.540000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -961,7 +967,7 @@
         <v>17.87</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="37" t="s">
         <v>22</v>
       </c>
@@ -979,7 +985,7 @@
         <v>8.48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="19" t="s">
         <v>23</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>7.4300000000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="19" t="s">
         <v>24</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="19" t="s">
         <v>25</v>
       </c>
@@ -1026,12 +1032,14 @@
       <c r="D15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>44</v>
+      </c>
       <c r="F15" s="18">
         <v>3.51</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="19" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1057,7 @@
         <v>6.4999999999999991</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75">
       <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
@@ -1060,12 +1068,14 @@
       <c r="D17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <v>20.05</v>
+      </c>
       <c r="F17">
         <v>4.7800000000000011</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.75">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -1073,7 +1083,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
@@ -1081,7 +1091,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
@@ -1089,7 +1099,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -1097,7 +1107,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="4"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -1105,7 +1115,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -1113,7 +1123,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15.75">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
@@ -1121,7 +1131,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15.75">
       <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
@@ -1142,14 +1152,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="15.75">
       <c r="A2" s="21">
         <v>0</v>
       </c>
@@ -1165,12 +1175,12 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="15.75">
       <c r="A3" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="15.75">
       <c r="A4" s="21">
         <v>9</v>
       </c>
@@ -1187,7 +1197,7 @@
       <c r="W4" s="21"/>
       <c r="X4" s="21"/>
     </row>
-    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="15.75">
       <c r="A5" s="21">
         <v>16</v>
       </c>
@@ -1204,7 +1214,7 @@
       <c r="W5" s="21"/>
       <c r="X5" s="21"/>
     </row>
-    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="15.75">
       <c r="A6" s="21">
         <v>23</v>
       </c>
@@ -1221,7 +1231,7 @@
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
     </row>
-    <row r="7" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="15.75">
       <c r="A7" s="21">
         <v>30</v>
       </c>
@@ -1238,7 +1248,7 @@
       <c r="W7" s="21"/>
       <c r="X7" s="21"/>
     </row>
-    <row r="8" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="15.75">
       <c r="A8" s="21">
         <v>56</v>
       </c>
@@ -1255,7 +1265,7 @@
       <c r="W8" s="21"/>
       <c r="X8" s="21"/>
     </row>
-    <row r="9" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="15.75">
       <c r="A9" s="21">
         <v>72</v>
       </c>
@@ -1272,7 +1282,7 @@
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
     </row>
-    <row r="10" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="15.75">
       <c r="A10" s="21">
         <v>83</v>
       </c>
@@ -1289,7 +1299,7 @@
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
     </row>
-    <row r="11" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="15.75">
       <c r="A11" s="21">
         <v>99</v>
       </c>
@@ -1306,7 +1316,7 @@
       <c r="W11" s="21"/>
       <c r="X11" s="21"/>
     </row>
-    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="15.75">
       <c r="A12" s="21">
         <v>126</v>
       </c>
@@ -1323,7 +1333,7 @@
       <c r="W12" s="21"/>
       <c r="X12" s="21"/>
     </row>
-    <row r="13" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="15.75">
       <c r="A13" s="21">
         <v>150</v>
       </c>
@@ -1340,7 +1350,7 @@
       <c r="W13" s="21"/>
       <c r="X13" s="21"/>
     </row>
-    <row r="14" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="15.75">
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
       <c r="O14" s="21"/>
@@ -1354,7 +1364,7 @@
       <c r="W14" s="21"/>
       <c r="X14" s="21"/>
     </row>
-    <row r="15" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="15.75">
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
       <c r="O15" s="21"/>
@@ -1381,9 +1391,9 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -1437,7 +1447,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
@@ -1492,7 +1502,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +1557,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
@@ -1599,7 +1609,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
@@ -1651,7 +1661,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75">
       <c r="A6" s="19" t="s">
         <v>17</v>
       </c>
@@ -1706,7 +1716,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>18</v>
       </c>
@@ -1761,7 +1771,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75">
       <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
@@ -1816,7 +1826,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
@@ -1871,7 +1881,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -1926,7 +1936,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -1981,7 +1991,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
@@ -2036,7 +2046,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75">
       <c r="A13" s="19" t="s">
         <v>24</v>
       </c>
@@ -2091,7 +2101,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75">
       <c r="A14" s="19" t="s">
         <v>25</v>
       </c>
@@ -2146,7 +2156,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="19" t="s">
         <v>26</v>
       </c>
@@ -2201,7 +2211,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -2255,7 +2265,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -2272,7 +2282,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15.75">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -2289,7 +2299,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -2306,7 +2316,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -2323,7 +2333,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -2340,7 +2350,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
@@ -2357,7 +2367,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -2374,7 +2384,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
@@ -2404,9 +2414,9 @@
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16.5" thickBot="1">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -2441,7 +2451,7 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
@@ -2476,7 +2486,7 @@
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -2511,7 +2521,7 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
@@ -2546,7 +2556,7 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
@@ -2581,7 +2591,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="16.5" thickBot="1">
       <c r="A6" s="19" t="s">
         <v>17</v>
       </c>
@@ -2616,7 +2626,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>18</v>
       </c>
@@ -2651,7 +2661,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16.5" thickBot="1">
       <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2696,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
@@ -2721,7 +2731,7 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="16.5" thickBot="1">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -2756,7 +2766,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -2791,7 +2801,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
@@ -2826,7 +2836,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="16.5" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>24</v>
       </c>
@@ -2861,7 +2871,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
     </row>
-    <row r="14" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="16.5" thickBot="1">
       <c r="A14" s="19" t="s">
         <v>25</v>
       </c>
@@ -2896,7 +2906,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="19" t="s">
         <v>26</v>
       </c>
@@ -2931,7 +2941,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -2966,7 +2976,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75">
       <c r="A17" s="2"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2983,7 +2993,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15.75">
       <c r="A18" s="2"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3000,7 +3010,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75">
       <c r="A19" s="2"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -3017,7 +3027,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75">
       <c r="A20" s="2"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3034,7 +3044,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75">
       <c r="A21" s="2"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -3051,7 +3061,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75">
       <c r="A22" s="2"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -3068,7 +3078,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75">
       <c r="A23" s="2"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -3085,7 +3095,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75">
       <c r="A24" s="2"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3115,9 +3125,9 @@
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -3172,7 +3182,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
@@ -3227,7 +3237,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -3282,7 +3292,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
@@ -3334,7 +3344,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
@@ -3386,7 +3396,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75">
       <c r="A6" s="19" t="s">
         <v>17</v>
       </c>
@@ -3441,7 +3451,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="19" t="s">
         <v>18</v>
       </c>
@@ -3496,7 +3506,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75">
       <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
@@ -3551,7 +3561,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
@@ -3606,7 +3616,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -3661,7 +3671,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -3716,7 +3726,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
@@ -3771,7 +3781,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75">
       <c r="A13" s="19" t="s">
         <v>24</v>
       </c>
@@ -3826,7 +3836,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75">
       <c r="A14" s="19" t="s">
         <v>25</v>
       </c>
@@ -3881,7 +3891,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="19" t="s">
         <v>26</v>
       </c>
@@ -3936,7 +3946,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -3991,7 +4001,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75">
       <c r="A17" s="2"/>
       <c r="B17" s="12"/>
       <c r="C17" s="14"/>
@@ -4008,7 +4018,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15.75">
       <c r="A18" s="2"/>
       <c r="B18" s="12"/>
       <c r="C18" s="14"/>
@@ -4025,7 +4035,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75">
       <c r="A19" s="2"/>
       <c r="B19" s="12"/>
       <c r="C19" s="14"/>
@@ -4042,7 +4052,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75">
       <c r="A20" s="2"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -4059,7 +4069,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="14"/>
@@ -4076,7 +4086,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75">
       <c r="A22" s="2"/>
       <c r="B22" s="12"/>
       <c r="C22" s="14"/>
@@ -4093,7 +4103,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75">
       <c r="A23" s="2"/>
       <c r="B23" s="6"/>
       <c r="C23" s="14"/>
@@ -4110,7 +4120,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="13"/>

</xml_diff>

<commit_message>
separate analysis per experiment and refinements of the plots
</commit_message>
<xml_diff>
--- a/data/exp_raw/johann_batch_preprocessed_part2.xlsx
+++ b/data/exp_raw/johann_batch_preprocessed_part2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcant\Documents\AmmerBatch\data\exp_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329EE3A7-BE36-4362-8A0F-B52F4B8148F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E88313-6564-4457-8261-25EFFCD12023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14910" yWindow="2085" windowWidth="8580" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -909,10 +909,10 @@
         <v>28</v>
       </c>
       <c r="E8" s="39">
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="F8" s="40">
-        <v>3.0100000000000007</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75">
@@ -926,9 +926,11 @@
       <c r="D9" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="39">
+        <v>42.6</v>
+      </c>
       <c r="F9" s="40">
-        <v>3.6100000000000003</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75">
@@ -943,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="41">
-        <v>3.7</v>
+        <v>3.67</v>
       </c>
       <c r="F10" s="18">
         <v>15.540000000000003</v>
@@ -1036,7 +1038,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="18">
-        <v>3.51</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75">

</xml_diff>